<commit_message>
add save column in s_vals sheets
</commit_message>
<xml_diff>
--- a/data/s_vals/2021/abad_fernando.xlsx
+++ b/data/s_vals/2021/abad_fernando.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>sum</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Save</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -489,6 +494,9 @@
       <c r="G2" t="n">
         <v>3.536033448013082</v>
       </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -513,6 +521,9 @@
       </c>
       <c r="G3" t="n">
         <v>6.15379541431027</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>